<commit_message>
learning(my app with register, login, hash password comparing, download, upload, works with sql, excel works) I have added a possibility to enter column name for which you want to make subtraction, plussing or any other thing.
</commit_message>
<xml_diff>
--- a/downloads/newDataFile2.xlsx
+++ b/downloads/newDataFile2.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -398,7 +398,7 @@
         <v>state</v>
       </c>
       <c r="F1" t="str">
-        <v>saleWithoutCosts</v>
+        <v>newColumn</v>
       </c>
     </row>
     <row r="2">
@@ -406,7 +406,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>44145.028449074074</v>
+        <v>44146.03377314815</v>
       </c>
       <c r="C2" t="str">
         <v>Alaska</v>
@@ -418,7 +418,7 @@
         <v>NY</v>
       </c>
       <c r="F2">
-        <v>-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -426,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>44145.028449074074</v>
+        <v>44146.03377314815</v>
       </c>
       <c r="C3" t="str">
         <v>Illinois</v>
@@ -438,7 +438,7 @@
         <v>IL</v>
       </c>
       <c r="F3">
-        <v>-8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -446,7 +446,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>44145.028449074074</v>
+        <v>44146.03377314815</v>
       </c>
       <c r="C4" t="str">
         <v>Toronto</v>
@@ -458,7 +458,7 @@
         <v>OH</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -466,7 +466,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>44145.028449074074</v>
+        <v>44146.03377314815</v>
       </c>
       <c r="C5" t="str">
         <v>Pensilvania</v>
@@ -478,7 +478,7 @@
         <v>NV</v>
       </c>
       <c r="F5">
-        <v>203</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -486,7 +486,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>44145.028449074074</v>
+        <v>44146.03377314815</v>
       </c>
       <c r="C6" t="str">
         <v>D.C. Columbia</v>
@@ -498,12 +498,112 @@
         <v>CA</v>
       </c>
       <c r="F6">
-        <v>206</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44146.03579861111</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Alaska</v>
+      </c>
+      <c r="D7" t="str">
+        <v>ADIDAS</v>
+      </c>
+      <c r="E7" t="str">
+        <v>NY</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44146.03579861111</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Illinois</v>
+      </c>
+      <c r="D8" t="str">
+        <v>NEW BALANCE</v>
+      </c>
+      <c r="E8" t="str">
+        <v>IL</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44146.03579861111</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Toronto</v>
+      </c>
+      <c r="D9" t="str">
+        <v>TOMMY HILFIGER</v>
+      </c>
+      <c r="E9" t="str">
+        <v>OH</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44146.03579861111</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Pensilvania</v>
+      </c>
+      <c r="D10" t="str">
+        <v>M TAC</v>
+      </c>
+      <c r="E10" t="str">
+        <v>NV</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44146.03579861111</v>
+      </c>
+      <c r="C11" t="str">
+        <v>D.C. Columbia</v>
+      </c>
+      <c r="D11" t="str">
+        <v>five eleven</v>
+      </c>
+      <c r="E11" t="str">
+        <v>CA</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
learning(myapp) I have added a better styles to pages, so now it looks very nice and user friendly I have added a Jmeter test of this app which has been recorded by Jmeter
</commit_message>
<xml_diff>
--- a/downloads/newDataFile2.xlsx
+++ b/downloads/newDataFile2.xlsx
@@ -42,9 +42,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,234 +375,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>id</v>
-      </c>
-      <c r="B1" t="str">
-        <v>added_date</v>
-      </c>
-      <c r="C1" t="str">
-        <v>region</v>
-      </c>
-      <c r="D1" t="str">
-        <v>brand</v>
-      </c>
-      <c r="E1" t="str">
-        <v>state</v>
-      </c>
-      <c r="F1" t="str">
-        <v>newColumn</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44146.03377314815</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Alaska</v>
-      </c>
-      <c r="D2" t="str">
-        <v>ADIDAS</v>
-      </c>
-      <c r="E2" t="str">
-        <v>NY</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44146.03377314815</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Illinois</v>
-      </c>
-      <c r="D3" t="str">
-        <v>NEW BALANCE</v>
-      </c>
-      <c r="E3" t="str">
-        <v>IL</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44146.03377314815</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Toronto</v>
-      </c>
-      <c r="D4" t="str">
-        <v>TOMMY HILFIGER</v>
-      </c>
-      <c r="E4" t="str">
-        <v>OH</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44146.03377314815</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Pensilvania</v>
-      </c>
-      <c r="D5" t="str">
-        <v>M TAC</v>
-      </c>
-      <c r="E5" t="str">
-        <v>NV</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>44146.03377314815</v>
-      </c>
-      <c r="C6" t="str">
-        <v>D.C. Columbia</v>
-      </c>
-      <c r="D6" t="str">
-        <v>five eleven</v>
-      </c>
-      <c r="E6" t="str">
-        <v>CA</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44146.03579861111</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Alaska</v>
-      </c>
-      <c r="D7" t="str">
-        <v>ADIDAS</v>
-      </c>
-      <c r="E7" t="str">
-        <v>NY</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44146.03579861111</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Illinois</v>
-      </c>
-      <c r="D8" t="str">
-        <v>NEW BALANCE</v>
-      </c>
-      <c r="E8" t="str">
-        <v>IL</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>44146.03579861111</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Toronto</v>
-      </c>
-      <c r="D9" t="str">
-        <v>TOMMY HILFIGER</v>
-      </c>
-      <c r="E9" t="str">
-        <v>OH</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1">
-        <v>44146.03579861111</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Pensilvania</v>
-      </c>
-      <c r="D10" t="str">
-        <v>M TAC</v>
-      </c>
-      <c r="E10" t="str">
-        <v>NV</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1">
-        <v>44146.03579861111</v>
-      </c>
-      <c r="C11" t="str">
-        <v>D.C. Columbia</v>
-      </c>
-      <c r="D11" t="str">
-        <v>five eleven</v>
-      </c>
-      <c r="E11" t="str">
-        <v>CA</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>